<commit_message>
Working on class hierarchy
ExcelBook
TKE
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DF5221-007A-4895-83F3-8D0AE160FED5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1634BD-283C-4496-A34C-7EC6D390DB96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1368" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,15 +574,15 @@
       </c>
       <c r="I12">
         <f ca="1">J12+K12</f>
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J12">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="K12" s="2">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>48</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -612,15 +612,15 @@
       </c>
       <c r="I13" s="2">
         <f t="shared" ref="I13:I22" ca="1" si="0">J13+K13</f>
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" ref="J13:L22" ca="1" si="1">RANDBETWEEN(1, 100)</f>
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -650,15 +650,15 @@
       </c>
       <c r="I14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -685,15 +685,15 @@
       </c>
       <c r="I15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -717,15 +717,15 @@
       </c>
       <c r="I16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="2"/>
     </row>
@@ -753,15 +753,15 @@
       </c>
       <c r="I17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -788,15 +788,15 @@
       </c>
       <c r="I18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -820,15 +820,15 @@
       </c>
       <c r="I19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -852,15 +852,15 @@
       </c>
       <c r="I20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -884,15 +884,15 @@
       </c>
       <c r="I21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -916,15 +916,15 @@
       </c>
       <c r="I22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on formula translation
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1634BD-283C-4496-A34C-7EC6D390DB96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF164165-D005-4CAF-BF2A-5ABEE87DE135}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1368" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7476" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -129,12 +131,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -157,6 +189,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -437,117 +478,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L22"/>
+  <dimension ref="A2:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3" t="s">
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-      <c r="I7" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="3"/>
+      <c r="J7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>27</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -572,20 +618,24 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <f ca="1">J12+K12</f>
-        <v>131</v>
+      <c r="I12" s="4">
+        <f ca="1">5+J12</f>
+        <v>92</v>
       </c>
       <c r="J12">
+        <f ca="1">SUM(K12:L12)</f>
+        <v>87</v>
+      </c>
+      <c r="K12">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>41</v>
-      </c>
-      <c r="K12" s="2">
+        <v>40</v>
+      </c>
+      <c r="L12" s="2">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -610,20 +660,24 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="2">
-        <f t="shared" ref="I13:I22" ca="1" si="0">J13+K13</f>
-        <v>68</v>
-      </c>
-      <c r="J13" s="2">
-        <f t="shared" ref="J13:L22" ca="1" si="1">RANDBETWEEN(1, 100)</f>
-        <v>64</v>
+      <c r="I13" s="4">
+        <f t="shared" ref="I13:I22" ca="1" si="0">5+J13</f>
+        <v>160</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ref="J13:J22" ca="1" si="1">SUM(K13:L13)</f>
+        <v>155</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K13:L22" ca="1" si="2">RANDBETWEEN(1, 100)</f>
+        <v>78</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -648,20 +702,24 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="J14" s="2">
+        <v>138</v>
+      </c>
+      <c r="J14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -683,20 +741,24 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>137</v>
-      </c>
-      <c r="J15" s="2">
+        <v>167</v>
+      </c>
+      <c r="J15" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -715,21 +777,25 @@
       <c r="H16" s="1">
         <v>0</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="J16" s="2">
+        <v>78</v>
+      </c>
+      <c r="J16" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -751,20 +817,24 @@
       <c r="H17" s="1">
         <v>0</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="J17" s="2">
+        <v>124</v>
+      </c>
+      <c r="J17" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -786,20 +856,24 @@
       <c r="H18" s="1">
         <v>0</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="J18" s="2">
+        <v>46</v>
+      </c>
+      <c r="J18" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -818,20 +892,24 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="J19" s="2">
+        <v>57</v>
+      </c>
+      <c r="J19" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -850,20 +928,24 @@
       <c r="H20" s="1">
         <v>0</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="J20" s="2">
+        <v>79</v>
+      </c>
+      <c r="J20" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -882,20 +964,24 @@
       <c r="H21" s="1">
         <v>0</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="J21" s="2">
+        <v>118</v>
+      </c>
+      <c r="J21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -914,23 +1000,27 @@
       <c r="H22" s="1">
         <v>0</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>119</v>
-      </c>
-      <c r="J22" s="2">
+        <v>82</v>
+      </c>
+      <c r="J22" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="J5:L6"/>
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
@@ -943,4 +1033,135 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFE1558-6EAD-40FB-93D6-9619E326BF93}">
+  <dimension ref="B2:M19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G18" s="9"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on updating formulas
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF164165-D005-4CAF-BF2A-5ABEE87DE135}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF899CA5-A975-43EE-9E0F-F7613765AF9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7476" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <dimension ref="A2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,19 +620,19 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">5+J12</f>
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="J12">
         <f ca="1">SUM(K12:L12)</f>
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="K12">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="L12" s="2">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -662,19 +662,19 @@
       </c>
       <c r="I13" s="4">
         <f t="shared" ref="I13:I22" ca="1" si="0">5+J13</f>
-        <v>160</v>
+        <v>83</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" ref="J13:J22" ca="1" si="1">SUM(K13:L13)</f>
-        <v>155</v>
+        <v>78</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" ref="K13:L22" ca="1" si="2">RANDBETWEEN(1, 100)</f>
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>77</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -704,19 +704,19 @@
       </c>
       <c r="I14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -743,19 +743,19 @@
       </c>
       <c r="I15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>62</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -779,19 +779,19 @@
       </c>
       <c r="I16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="M16" s="2"/>
     </row>
@@ -819,19 +819,19 @@
       </c>
       <c r="I17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -858,19 +858,19 @@
       </c>
       <c r="I18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -894,19 +894,19 @@
       </c>
       <c r="I19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -930,19 +930,19 @@
       </c>
       <c r="I20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -966,19 +966,19 @@
       </c>
       <c r="I21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1002,19 +1002,19 @@
       </c>
       <c r="I22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>